<commit_message>
01.Trabajo Practico Primera Entrega ejemplo
01.Trabajo Practico Primera Entrega ejemplo Listo para revisión
</commit_message>
<xml_diff>
--- a/Introducción a los Sistemas Operativos/Trabajos Prácticos/Resultados.xlsx
+++ b/Introducción a los Sistemas Operativos/Trabajos Prácticos/Resultados.xlsx
@@ -285,6 +285,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -304,9 +307,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -589,8 +589,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BA51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="T42" sqref="T42"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="AD30" sqref="AD30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -601,35 +601,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:53" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="24" t="s">
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="25" t="s">
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="23" t="s">
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="O1" s="23"/>
-      <c r="P1" s="23"/>
-      <c r="Q1" s="26" t="s">
+      <c r="O1" s="24"/>
+      <c r="P1" s="24"/>
+      <c r="Q1" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="R1" s="26"/>
-      <c r="S1" s="26"/>
+      <c r="R1" s="27"/>
+      <c r="S1" s="27"/>
       <c r="T1" s="2"/>
       <c r="U1" s="2"/>
       <c r="V1" s="2"/>
@@ -652,31 +652,31 @@
       <c r="AM1" s="1"/>
     </row>
     <row r="2" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="A2" s="23"/>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="25" t="s">
+      <c r="A2" s="24"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25" t="s">
+      <c r="I2" s="26"/>
+      <c r="J2" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="25"/>
-      <c r="L2" s="25" t="s">
+      <c r="K2" s="26"/>
+      <c r="L2" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="M2" s="25"/>
-      <c r="N2" s="23"/>
-      <c r="O2" s="23"/>
-      <c r="P2" s="23"/>
-      <c r="Q2" s="26"/>
-      <c r="R2" s="26"/>
-      <c r="S2" s="26"/>
+      <c r="M2" s="26"/>
+      <c r="N2" s="24"/>
+      <c r="O2" s="24"/>
+      <c r="P2" s="24"/>
+      <c r="Q2" s="27"/>
+      <c r="R2" s="27"/>
+      <c r="S2" s="27"/>
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
       <c r="V2" s="1"/>
@@ -699,40 +699,40 @@
       <c r="AM2" s="1"/>
     </row>
     <row r="3" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21" t="s">
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21">
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22">
         <v>4</v>
       </c>
-      <c r="I3" s="21"/>
-      <c r="J3" s="21">
+      <c r="I3" s="22"/>
+      <c r="J3" s="22">
         <v>2</v>
       </c>
-      <c r="K3" s="21"/>
-      <c r="L3" s="21">
+      <c r="K3" s="22"/>
+      <c r="L3" s="22">
         <v>3</v>
       </c>
-      <c r="M3" s="21"/>
-      <c r="N3" s="21" t="s">
+      <c r="M3" s="22"/>
+      <c r="N3" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="O3" s="21"/>
-      <c r="P3" s="21"/>
-      <c r="Q3" s="22">
+      <c r="O3" s="22"/>
+      <c r="P3" s="22"/>
+      <c r="Q3" s="23">
         <f>SUM(H3,L3)</f>
         <v>7</v>
       </c>
-      <c r="R3" s="22"/>
-      <c r="S3" s="22"/>
+      <c r="R3" s="23"/>
+      <c r="S3" s="23"/>
       <c r="T3" s="1"/>
       <c r="U3" s="1"/>
       <c r="V3" s="1"/>
@@ -755,40 +755,40 @@
       <c r="AM3" s="1"/>
     </row>
     <row r="4" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="21"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21" t="s">
+      <c r="B4" s="22"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21">
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22">
         <v>3</v>
       </c>
-      <c r="I4" s="21"/>
-      <c r="J4" s="21">
+      <c r="I4" s="22"/>
+      <c r="J4" s="22">
         <v>4</v>
       </c>
-      <c r="K4" s="21"/>
-      <c r="L4" s="21">
+      <c r="K4" s="22"/>
+      <c r="L4" s="22">
         <v>3</v>
       </c>
-      <c r="M4" s="21"/>
-      <c r="N4" s="21" t="s">
+      <c r="M4" s="22"/>
+      <c r="N4" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="O4" s="21"/>
-      <c r="P4" s="21"/>
-      <c r="Q4" s="22">
+      <c r="O4" s="22"/>
+      <c r="P4" s="22"/>
+      <c r="Q4" s="23">
         <f t="shared" ref="Q4:Q9" si="0">SUM(H4,L4)</f>
         <v>6</v>
       </c>
-      <c r="R4" s="22"/>
-      <c r="S4" s="22"/>
+      <c r="R4" s="23"/>
+      <c r="S4" s="23"/>
       <c r="T4" s="1"/>
       <c r="U4" s="1"/>
       <c r="V4" s="1"/>
@@ -811,40 +811,40 @@
       <c r="AM4" s="1"/>
     </row>
     <row r="5" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21" t="s">
+      <c r="B5" s="22"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="21">
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22">
         <v>2</v>
       </c>
-      <c r="I5" s="21"/>
-      <c r="J5" s="21">
+      <c r="I5" s="22"/>
+      <c r="J5" s="22">
         <v>2</v>
       </c>
-      <c r="K5" s="21"/>
-      <c r="L5" s="21">
+      <c r="K5" s="22"/>
+      <c r="L5" s="22">
         <v>6</v>
       </c>
-      <c r="M5" s="21"/>
-      <c r="N5" s="21" t="s">
+      <c r="M5" s="22"/>
+      <c r="N5" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="O5" s="21"/>
-      <c r="P5" s="21"/>
-      <c r="Q5" s="22">
+      <c r="O5" s="22"/>
+      <c r="P5" s="22"/>
+      <c r="Q5" s="23">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="R5" s="22"/>
-      <c r="S5" s="22"/>
+      <c r="R5" s="23"/>
+      <c r="S5" s="23"/>
       <c r="T5" s="1"/>
       <c r="U5" s="1"/>
       <c r="V5" s="1"/>
@@ -867,40 +867,40 @@
       <c r="AM5" s="1"/>
     </row>
     <row r="6" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="21"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21" t="s">
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
-      <c r="H6" s="21">
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22">
         <v>1</v>
       </c>
-      <c r="I6" s="21"/>
-      <c r="J6" s="21">
+      <c r="I6" s="22"/>
+      <c r="J6" s="22">
         <v>3</v>
       </c>
-      <c r="K6" s="21"/>
-      <c r="L6" s="21">
+      <c r="K6" s="22"/>
+      <c r="L6" s="22">
         <v>2</v>
       </c>
-      <c r="M6" s="21"/>
-      <c r="N6" s="21" t="s">
+      <c r="M6" s="22"/>
+      <c r="N6" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="O6" s="21"/>
-      <c r="P6" s="21"/>
-      <c r="Q6" s="22">
+      <c r="O6" s="22"/>
+      <c r="P6" s="22"/>
+      <c r="Q6" s="23">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="R6" s="22"/>
-      <c r="S6" s="22"/>
+      <c r="R6" s="23"/>
+      <c r="S6" s="23"/>
       <c r="T6" s="1"/>
       <c r="U6" s="1"/>
       <c r="V6" s="1"/>
@@ -923,40 +923,40 @@
       <c r="AM6" s="1"/>
     </row>
     <row r="7" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21" t="s">
+      <c r="B7" s="22"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="21">
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22">
         <v>1</v>
       </c>
-      <c r="I7" s="21"/>
-      <c r="J7" s="21">
+      <c r="I7" s="22"/>
+      <c r="J7" s="22">
         <v>1</v>
       </c>
-      <c r="K7" s="21"/>
-      <c r="L7" s="21">
+      <c r="K7" s="22"/>
+      <c r="L7" s="22">
         <v>5</v>
       </c>
-      <c r="M7" s="21"/>
-      <c r="N7" s="21" t="s">
+      <c r="M7" s="22"/>
+      <c r="N7" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="O7" s="21"/>
-      <c r="P7" s="21"/>
-      <c r="Q7" s="22">
+      <c r="O7" s="22"/>
+      <c r="P7" s="22"/>
+      <c r="Q7" s="23">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="R7" s="22"/>
-      <c r="S7" s="22"/>
+      <c r="R7" s="23"/>
+      <c r="S7" s="23"/>
       <c r="T7" s="1"/>
       <c r="U7" s="1"/>
       <c r="V7" s="1"/>
@@ -979,40 +979,40 @@
       <c r="AM7" s="1"/>
     </row>
     <row r="8" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="21"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21" t="s">
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21">
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22">
         <v>4</v>
       </c>
-      <c r="I8" s="21"/>
-      <c r="J8" s="21">
+      <c r="I8" s="22"/>
+      <c r="J8" s="22">
         <v>1</v>
       </c>
-      <c r="K8" s="21"/>
-      <c r="L8" s="21">
+      <c r="K8" s="22"/>
+      <c r="L8" s="22">
         <v>3</v>
       </c>
-      <c r="M8" s="21"/>
-      <c r="N8" s="21" t="s">
+      <c r="M8" s="22"/>
+      <c r="N8" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="O8" s="21"/>
-      <c r="P8" s="21"/>
-      <c r="Q8" s="22">
+      <c r="O8" s="22"/>
+      <c r="P8" s="22"/>
+      <c r="Q8" s="23">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="R8" s="22"/>
-      <c r="S8" s="22"/>
+      <c r="R8" s="23"/>
+      <c r="S8" s="23"/>
       <c r="T8" s="1"/>
       <c r="U8" s="1"/>
       <c r="V8" s="1"/>
@@ -1035,40 +1035,40 @@
       <c r="AM8" s="1"/>
     </row>
     <row r="9" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="A9" s="21" t="s">
+      <c r="A9" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21" t="s">
+      <c r="B9" s="22"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21">
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22">
         <v>5</v>
       </c>
-      <c r="I9" s="21"/>
-      <c r="J9" s="21">
+      <c r="I9" s="22"/>
+      <c r="J9" s="22">
         <v>2</v>
       </c>
-      <c r="K9" s="21"/>
-      <c r="L9" s="21">
+      <c r="K9" s="22"/>
+      <c r="L9" s="22">
         <v>1</v>
       </c>
-      <c r="M9" s="21"/>
-      <c r="N9" s="21" t="s">
+      <c r="M9" s="22"/>
+      <c r="N9" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="O9" s="21"/>
-      <c r="P9" s="21"/>
-      <c r="Q9" s="22">
+      <c r="O9" s="22"/>
+      <c r="P9" s="22"/>
+      <c r="Q9" s="23">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="R9" s="22"/>
-      <c r="S9" s="22"/>
+      <c r="R9" s="23"/>
+      <c r="S9" s="23"/>
       <c r="T9" s="1"/>
       <c r="U9" s="1"/>
       <c r="V9" s="1"/>
@@ -1091,40 +1091,40 @@
       <c r="AM9" s="1"/>
     </row>
     <row r="10" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="A10" s="21" t="s">
+      <c r="A10" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21" t="s">
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="21">
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22">
         <v>1</v>
       </c>
-      <c r="I10" s="21"/>
-      <c r="J10" s="21">
+      <c r="I10" s="22"/>
+      <c r="J10" s="22">
         <v>3</v>
       </c>
-      <c r="K10" s="21"/>
-      <c r="L10" s="21">
+      <c r="K10" s="22"/>
+      <c r="L10" s="22">
         <v>1</v>
       </c>
-      <c r="M10" s="21"/>
-      <c r="N10" s="21" t="s">
+      <c r="M10" s="22"/>
+      <c r="N10" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="O10" s="21"/>
-      <c r="P10" s="21"/>
-      <c r="Q10" s="22">
+      <c r="O10" s="22"/>
+      <c r="P10" s="22"/>
+      <c r="Q10" s="23">
         <f t="shared" ref="Q10" si="1">SUM(H10,L10)</f>
         <v>2</v>
       </c>
-      <c r="R10" s="22"/>
-      <c r="S10" s="22"/>
+      <c r="R10" s="23"/>
+      <c r="S10" s="23"/>
       <c r="T10" s="1"/>
       <c r="U10" s="1"/>
       <c r="V10" s="1"/>
@@ -1152,68 +1152,68 @@
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
-      <c r="D11" s="27" t="s">
+      <c r="D11" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="27"/>
-      <c r="H11" s="27"/>
-      <c r="I11" s="27"/>
-      <c r="J11" s="27"/>
-      <c r="K11" s="27"/>
-      <c r="L11" s="27"/>
-      <c r="M11" s="27"/>
-      <c r="N11" s="27"/>
-      <c r="O11" s="27"/>
-      <c r="P11" s="27"/>
-      <c r="Q11" s="27"/>
-      <c r="R11" s="27"/>
-      <c r="S11" s="27"/>
-      <c r="T11" s="27"/>
-      <c r="U11" s="27"/>
-      <c r="V11" s="27"/>
-      <c r="W11" s="27"/>
-      <c r="X11" s="27"/>
-      <c r="Y11" s="27"/>
-      <c r="Z11" s="27"/>
-      <c r="AA11" s="27"/>
-      <c r="AB11" s="27"/>
-      <c r="AC11" s="27"/>
-      <c r="AD11" s="27"/>
-      <c r="AE11" s="27"/>
-      <c r="AF11" s="27"/>
-      <c r="AG11" s="27"/>
-      <c r="AH11" s="27"/>
-      <c r="AI11" s="27"/>
-      <c r="AJ11" s="27"/>
-      <c r="AK11" s="27"/>
-      <c r="AL11" s="27"/>
-      <c r="AM11" s="27"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="28"/>
+      <c r="I11" s="28"/>
+      <c r="J11" s="28"/>
+      <c r="K11" s="28"/>
+      <c r="L11" s="28"/>
+      <c r="M11" s="28"/>
+      <c r="N11" s="28"/>
+      <c r="O11" s="28"/>
+      <c r="P11" s="28"/>
+      <c r="Q11" s="28"/>
+      <c r="R11" s="28"/>
+      <c r="S11" s="28"/>
+      <c r="T11" s="28"/>
+      <c r="U11" s="28"/>
+      <c r="V11" s="28"/>
+      <c r="W11" s="28"/>
+      <c r="X11" s="28"/>
+      <c r="Y11" s="28"/>
+      <c r="Z11" s="28"/>
+      <c r="AA11" s="28"/>
+      <c r="AB11" s="28"/>
+      <c r="AC11" s="28"/>
+      <c r="AD11" s="28"/>
+      <c r="AE11" s="28"/>
+      <c r="AF11" s="28"/>
+      <c r="AG11" s="28"/>
+      <c r="AH11" s="28"/>
+      <c r="AI11" s="28"/>
+      <c r="AJ11" s="28"/>
+      <c r="AK11" s="28"/>
+      <c r="AL11" s="28"/>
+      <c r="AM11" s="28"/>
     </row>
     <row r="12" spans="1:53" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="28">
+      <c r="B12" s="21">
         <v>1</v>
       </c>
-      <c r="C12" s="28">
+      <c r="C12" s="21">
         <v>2</v>
       </c>
-      <c r="D12" s="28">
+      <c r="D12" s="21">
         <v>3</v>
       </c>
-      <c r="E12" s="28">
+      <c r="E12" s="21">
         <v>4</v>
       </c>
-      <c r="F12" s="28">
+      <c r="F12" s="21">
         <v>5</v>
       </c>
       <c r="G12" s="4">
         <v>6</v>
       </c>
-      <c r="H12" s="28">
+      <c r="H12" s="21">
         <v>7</v>
       </c>
       <c r="I12" s="4">
@@ -2151,30 +2151,30 @@
       <c r="AM24" s="1"/>
     </row>
     <row r="25" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="A25" s="23" t="s">
+      <c r="A25" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B25" s="23"/>
-      <c r="C25" s="23"/>
-      <c r="D25" s="24" t="s">
+      <c r="B25" s="24"/>
+      <c r="C25" s="24"/>
+      <c r="D25" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="E25" s="24"/>
-      <c r="F25" s="24"/>
-      <c r="G25" s="24"/>
-      <c r="H25" s="25" t="s">
+      <c r="E25" s="25"/>
+      <c r="F25" s="25"/>
+      <c r="G25" s="25"/>
+      <c r="H25" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="I25" s="25"/>
-      <c r="J25" s="25"/>
-      <c r="K25" s="25"/>
-      <c r="L25" s="25"/>
-      <c r="M25" s="25"/>
-      <c r="N25" s="26" t="s">
+      <c r="I25" s="26"/>
+      <c r="J25" s="26"/>
+      <c r="K25" s="26"/>
+      <c r="L25" s="26"/>
+      <c r="M25" s="26"/>
+      <c r="N25" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="O25" s="26"/>
-      <c r="P25" s="26"/>
+      <c r="O25" s="27"/>
+      <c r="P25" s="27"/>
       <c r="Q25" s="14"/>
       <c r="R25" s="14"/>
       <c r="S25" s="14"/>
@@ -2200,28 +2200,28 @@
       <c r="AM25" s="1"/>
     </row>
     <row r="26" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="A26" s="23"/>
-      <c r="B26" s="23"/>
-      <c r="C26" s="23"/>
-      <c r="D26" s="24"/>
-      <c r="E26" s="24"/>
-      <c r="F26" s="24"/>
-      <c r="G26" s="24"/>
-      <c r="H26" s="25" t="s">
+      <c r="A26" s="24"/>
+      <c r="B26" s="24"/>
+      <c r="C26" s="24"/>
+      <c r="D26" s="25"/>
+      <c r="E26" s="25"/>
+      <c r="F26" s="25"/>
+      <c r="G26" s="25"/>
+      <c r="H26" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="I26" s="25"/>
-      <c r="J26" s="25" t="s">
+      <c r="I26" s="26"/>
+      <c r="J26" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="K26" s="25"/>
-      <c r="L26" s="25" t="s">
+      <c r="K26" s="26"/>
+      <c r="L26" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="M26" s="25"/>
-      <c r="N26" s="26"/>
-      <c r="O26" s="26"/>
-      <c r="P26" s="26"/>
+      <c r="M26" s="26"/>
+      <c r="N26" s="27"/>
+      <c r="O26" s="27"/>
+      <c r="P26" s="27"/>
       <c r="Q26" s="14"/>
       <c r="R26" s="14"/>
       <c r="S26" s="14"/>
@@ -2247,34 +2247,34 @@
       <c r="AM26" s="1"/>
     </row>
     <row r="27" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="A27" s="21" t="s">
+      <c r="A27" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B27" s="21"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="21" t="s">
+      <c r="B27" s="22"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="E27" s="21"/>
-      <c r="F27" s="21"/>
-      <c r="G27" s="21"/>
-      <c r="H27" s="21">
+      <c r="E27" s="22"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="22">
         <v>4</v>
       </c>
-      <c r="I27" s="21"/>
-      <c r="J27" s="21">
+      <c r="I27" s="22"/>
+      <c r="J27" s="22">
         <v>2</v>
       </c>
-      <c r="K27" s="21"/>
-      <c r="L27" s="21">
+      <c r="K27" s="22"/>
+      <c r="L27" s="22">
         <v>3</v>
       </c>
-      <c r="M27" s="21"/>
-      <c r="N27" s="22" t="s">
+      <c r="M27" s="22"/>
+      <c r="N27" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="O27" s="22"/>
-      <c r="P27" s="22"/>
+      <c r="O27" s="23"/>
+      <c r="P27" s="23"/>
       <c r="Q27" s="15"/>
       <c r="R27" s="15"/>
       <c r="S27" s="15"/>
@@ -2300,34 +2300,34 @@
       <c r="AM27" s="1"/>
     </row>
     <row r="28" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="A28" s="21" t="s">
+      <c r="A28" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="B28" s="21"/>
-      <c r="C28" s="21"/>
-      <c r="D28" s="21" t="s">
+      <c r="B28" s="22"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="E28" s="21"/>
-      <c r="F28" s="21"/>
-      <c r="G28" s="21"/>
-      <c r="H28" s="21">
+      <c r="E28" s="22"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="22"/>
+      <c r="H28" s="22">
         <v>3</v>
       </c>
-      <c r="I28" s="21"/>
-      <c r="J28" s="21">
+      <c r="I28" s="22"/>
+      <c r="J28" s="22">
         <v>4</v>
       </c>
-      <c r="K28" s="21"/>
-      <c r="L28" s="21">
+      <c r="K28" s="22"/>
+      <c r="L28" s="22">
         <v>3</v>
       </c>
-      <c r="M28" s="21"/>
-      <c r="N28" s="22" t="s">
+      <c r="M28" s="22"/>
+      <c r="N28" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="O28" s="22"/>
-      <c r="P28" s="22"/>
+      <c r="O28" s="23"/>
+      <c r="P28" s="23"/>
       <c r="Q28" s="15"/>
       <c r="R28" s="15"/>
       <c r="S28" s="15"/>
@@ -2353,34 +2353,34 @@
       <c r="AM28" s="1"/>
     </row>
     <row r="29" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="A29" s="21" t="s">
+      <c r="A29" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="B29" s="21"/>
-      <c r="C29" s="21"/>
-      <c r="D29" s="21" t="s">
+      <c r="B29" s="22"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="E29" s="21"/>
-      <c r="F29" s="21"/>
-      <c r="G29" s="21"/>
-      <c r="H29" s="21">
+      <c r="E29" s="22"/>
+      <c r="F29" s="22"/>
+      <c r="G29" s="22"/>
+      <c r="H29" s="22">
         <v>2</v>
       </c>
-      <c r="I29" s="21"/>
-      <c r="J29" s="21">
+      <c r="I29" s="22"/>
+      <c r="J29" s="22">
         <v>2</v>
       </c>
-      <c r="K29" s="21"/>
-      <c r="L29" s="21">
+      <c r="K29" s="22"/>
+      <c r="L29" s="22">
         <v>6</v>
       </c>
-      <c r="M29" s="21"/>
-      <c r="N29" s="22" t="s">
+      <c r="M29" s="22"/>
+      <c r="N29" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="O29" s="22"/>
-      <c r="P29" s="22"/>
+      <c r="O29" s="23"/>
+      <c r="P29" s="23"/>
       <c r="Q29" s="15"/>
       <c r="R29" s="15"/>
       <c r="S29" s="15"/>
@@ -2406,34 +2406,34 @@
       <c r="AM29" s="1"/>
     </row>
     <row r="30" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="A30" s="21" t="s">
+      <c r="A30" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="21"/>
-      <c r="C30" s="21"/>
-      <c r="D30" s="21" t="s">
+      <c r="B30" s="22"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="E30" s="21"/>
-      <c r="F30" s="21"/>
-      <c r="G30" s="21"/>
-      <c r="H30" s="21">
+      <c r="E30" s="22"/>
+      <c r="F30" s="22"/>
+      <c r="G30" s="22"/>
+      <c r="H30" s="22">
         <v>1</v>
       </c>
-      <c r="I30" s="21"/>
-      <c r="J30" s="21">
+      <c r="I30" s="22"/>
+      <c r="J30" s="22">
         <v>3</v>
       </c>
-      <c r="K30" s="21"/>
-      <c r="L30" s="21">
+      <c r="K30" s="22"/>
+      <c r="L30" s="22">
         <v>2</v>
       </c>
-      <c r="M30" s="21"/>
-      <c r="N30" s="22" t="s">
+      <c r="M30" s="22"/>
+      <c r="N30" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="O30" s="22"/>
-      <c r="P30" s="22"/>
+      <c r="O30" s="23"/>
+      <c r="P30" s="23"/>
       <c r="Q30" s="15"/>
       <c r="R30" s="15"/>
       <c r="S30" s="15"/>
@@ -2459,34 +2459,34 @@
       <c r="AM30" s="1"/>
     </row>
     <row r="31" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="A31" s="21" t="s">
+      <c r="A31" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="B31" s="21"/>
-      <c r="C31" s="21"/>
-      <c r="D31" s="21" t="s">
+      <c r="B31" s="22"/>
+      <c r="C31" s="22"/>
+      <c r="D31" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="E31" s="21"/>
-      <c r="F31" s="21"/>
-      <c r="G31" s="21"/>
-      <c r="H31" s="21">
+      <c r="E31" s="22"/>
+      <c r="F31" s="22"/>
+      <c r="G31" s="22"/>
+      <c r="H31" s="22">
         <v>1</v>
       </c>
-      <c r="I31" s="21"/>
-      <c r="J31" s="21">
+      <c r="I31" s="22"/>
+      <c r="J31" s="22">
         <v>1</v>
       </c>
-      <c r="K31" s="21"/>
-      <c r="L31" s="21">
+      <c r="K31" s="22"/>
+      <c r="L31" s="22">
         <v>5</v>
       </c>
-      <c r="M31" s="21"/>
-      <c r="N31" s="22" t="s">
+      <c r="M31" s="22"/>
+      <c r="N31" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="O31" s="22"/>
-      <c r="P31" s="22"/>
+      <c r="O31" s="23"/>
+      <c r="P31" s="23"/>
       <c r="Q31" s="15"/>
       <c r="R31" s="15"/>
       <c r="S31" s="15"/>
@@ -2512,34 +2512,34 @@
       <c r="AM31" s="1"/>
     </row>
     <row r="32" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="A32" s="21" t="s">
+      <c r="A32" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="B32" s="21"/>
-      <c r="C32" s="21"/>
-      <c r="D32" s="21" t="s">
+      <c r="B32" s="22"/>
+      <c r="C32" s="22"/>
+      <c r="D32" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="E32" s="21"/>
-      <c r="F32" s="21"/>
-      <c r="G32" s="21"/>
-      <c r="H32" s="21">
+      <c r="E32" s="22"/>
+      <c r="F32" s="22"/>
+      <c r="G32" s="22"/>
+      <c r="H32" s="22">
         <v>4</v>
       </c>
-      <c r="I32" s="21"/>
-      <c r="J32" s="21">
+      <c r="I32" s="22"/>
+      <c r="J32" s="22">
         <v>1</v>
       </c>
-      <c r="K32" s="21"/>
-      <c r="L32" s="21">
+      <c r="K32" s="22"/>
+      <c r="L32" s="22">
         <v>3</v>
       </c>
-      <c r="M32" s="21"/>
-      <c r="N32" s="22" t="s">
+      <c r="M32" s="22"/>
+      <c r="N32" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="O32" s="22"/>
-      <c r="P32" s="22"/>
+      <c r="O32" s="23"/>
+      <c r="P32" s="23"/>
       <c r="Q32" s="15"/>
       <c r="R32" s="15"/>
       <c r="S32" s="15"/>
@@ -2565,34 +2565,34 @@
       <c r="AM32" s="1"/>
     </row>
     <row r="33" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="A33" s="21" t="s">
+      <c r="A33" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B33" s="21"/>
-      <c r="C33" s="21"/>
-      <c r="D33" s="21" t="s">
+      <c r="B33" s="22"/>
+      <c r="C33" s="22"/>
+      <c r="D33" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="E33" s="21"/>
-      <c r="F33" s="21"/>
-      <c r="G33" s="21"/>
-      <c r="H33" s="21">
+      <c r="E33" s="22"/>
+      <c r="F33" s="22"/>
+      <c r="G33" s="22"/>
+      <c r="H33" s="22">
         <v>5</v>
       </c>
-      <c r="I33" s="21"/>
-      <c r="J33" s="21">
+      <c r="I33" s="22"/>
+      <c r="J33" s="22">
         <v>2</v>
       </c>
-      <c r="K33" s="21"/>
-      <c r="L33" s="21">
+      <c r="K33" s="22"/>
+      <c r="L33" s="22">
         <v>1</v>
       </c>
-      <c r="M33" s="21"/>
-      <c r="N33" s="22" t="s">
+      <c r="M33" s="22"/>
+      <c r="N33" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="O33" s="22"/>
-      <c r="P33" s="22"/>
+      <c r="O33" s="23"/>
+      <c r="P33" s="23"/>
       <c r="Q33" s="15"/>
       <c r="R33" s="15"/>
       <c r="S33" s="15"/>
@@ -2618,34 +2618,34 @@
       <c r="AM33" s="1"/>
     </row>
     <row r="34" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="A34" s="21" t="s">
+      <c r="A34" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B34" s="21"/>
-      <c r="C34" s="21"/>
-      <c r="D34" s="21" t="s">
+      <c r="B34" s="22"/>
+      <c r="C34" s="22"/>
+      <c r="D34" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="E34" s="21"/>
-      <c r="F34" s="21"/>
-      <c r="G34" s="21"/>
-      <c r="H34" s="21">
+      <c r="E34" s="22"/>
+      <c r="F34" s="22"/>
+      <c r="G34" s="22"/>
+      <c r="H34" s="22">
         <v>1</v>
       </c>
-      <c r="I34" s="21"/>
-      <c r="J34" s="21">
+      <c r="I34" s="22"/>
+      <c r="J34" s="22">
         <v>3</v>
       </c>
-      <c r="K34" s="21"/>
-      <c r="L34" s="21">
+      <c r="K34" s="22"/>
+      <c r="L34" s="22">
         <v>1</v>
       </c>
-      <c r="M34" s="21"/>
-      <c r="N34" s="22" t="s">
+      <c r="M34" s="22"/>
+      <c r="N34" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="O34" s="22"/>
-      <c r="P34" s="22"/>
+      <c r="O34" s="23"/>
+      <c r="P34" s="23"/>
       <c r="Q34" s="1"/>
       <c r="R34" s="1"/>
       <c r="S34" s="1"/>
@@ -2676,68 +2676,68 @@
       </c>
       <c r="B35" s="7"/>
       <c r="C35" s="7"/>
-      <c r="D35" s="27" t="s">
+      <c r="D35" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="E35" s="27"/>
-      <c r="F35" s="27"/>
-      <c r="G35" s="27"/>
-      <c r="H35" s="27"/>
-      <c r="I35" s="27"/>
-      <c r="J35" s="27"/>
-      <c r="K35" s="27"/>
-      <c r="L35" s="27"/>
-      <c r="M35" s="27"/>
-      <c r="N35" s="27"/>
-      <c r="O35" s="27"/>
-      <c r="P35" s="27"/>
-      <c r="Q35" s="27"/>
-      <c r="R35" s="27"/>
-      <c r="S35" s="27"/>
-      <c r="T35" s="27"/>
-      <c r="U35" s="27"/>
-      <c r="V35" s="27"/>
-      <c r="W35" s="27"/>
-      <c r="X35" s="27"/>
-      <c r="Y35" s="27"/>
-      <c r="Z35" s="27"/>
-      <c r="AA35" s="27"/>
-      <c r="AB35" s="27"/>
-      <c r="AC35" s="27"/>
-      <c r="AD35" s="27"/>
-      <c r="AE35" s="27"/>
-      <c r="AF35" s="27"/>
-      <c r="AG35" s="27"/>
-      <c r="AH35" s="27"/>
-      <c r="AI35" s="27"/>
-      <c r="AJ35" s="27"/>
-      <c r="AK35" s="27"/>
-      <c r="AL35" s="27"/>
-      <c r="AM35" s="27"/>
+      <c r="E35" s="28"/>
+      <c r="F35" s="28"/>
+      <c r="G35" s="28"/>
+      <c r="H35" s="28"/>
+      <c r="I35" s="28"/>
+      <c r="J35" s="28"/>
+      <c r="K35" s="28"/>
+      <c r="L35" s="28"/>
+      <c r="M35" s="28"/>
+      <c r="N35" s="28"/>
+      <c r="O35" s="28"/>
+      <c r="P35" s="28"/>
+      <c r="Q35" s="28"/>
+      <c r="R35" s="28"/>
+      <c r="S35" s="28"/>
+      <c r="T35" s="28"/>
+      <c r="U35" s="28"/>
+      <c r="V35" s="28"/>
+      <c r="W35" s="28"/>
+      <c r="X35" s="28"/>
+      <c r="Y35" s="28"/>
+      <c r="Z35" s="28"/>
+      <c r="AA35" s="28"/>
+      <c r="AB35" s="28"/>
+      <c r="AC35" s="28"/>
+      <c r="AD35" s="28"/>
+      <c r="AE35" s="28"/>
+      <c r="AF35" s="28"/>
+      <c r="AG35" s="28"/>
+      <c r="AH35" s="28"/>
+      <c r="AI35" s="28"/>
+      <c r="AJ35" s="28"/>
+      <c r="AK35" s="28"/>
+      <c r="AL35" s="28"/>
+      <c r="AM35" s="28"/>
     </row>
     <row r="36" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B36" s="28">
+      <c r="B36" s="21">
         <v>1</v>
       </c>
-      <c r="C36" s="28">
+      <c r="C36" s="21">
         <v>2</v>
       </c>
-      <c r="D36" s="28">
+      <c r="D36" s="21">
         <v>3</v>
       </c>
-      <c r="E36" s="28">
+      <c r="E36" s="21">
         <v>4</v>
       </c>
-      <c r="F36" s="28">
+      <c r="F36" s="21">
         <v>5</v>
       </c>
       <c r="G36" s="20">
         <v>6</v>
       </c>
-      <c r="H36" s="28">
+      <c r="H36" s="21">
         <v>7</v>
       </c>
       <c r="I36" s="4">
@@ -3780,6 +3780,17 @@
     <mergeCell ref="J34:K34"/>
     <mergeCell ref="L34:M34"/>
     <mergeCell ref="N34:P34"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="J26:K26"/>
+    <mergeCell ref="L26:M26"/>
+    <mergeCell ref="D11:AM11"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="D27:G27"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="L27:M27"/>
+    <mergeCell ref="N27:P27"/>
+    <mergeCell ref="A28:C28"/>
     <mergeCell ref="D35:AM35"/>
     <mergeCell ref="A1:C2"/>
     <mergeCell ref="D1:G2"/>
@@ -3820,9 +3831,7 @@
     <mergeCell ref="J6:K6"/>
     <mergeCell ref="L6:M6"/>
     <mergeCell ref="A7:C7"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="J26:K26"/>
-    <mergeCell ref="L26:M26"/>
+    <mergeCell ref="L8:M8"/>
     <mergeCell ref="Q3:S3"/>
     <mergeCell ref="Q4:S4"/>
     <mergeCell ref="Q5:S5"/>
@@ -3832,16 +3841,7 @@
     <mergeCell ref="N8:P8"/>
     <mergeCell ref="N5:P5"/>
     <mergeCell ref="N3:P3"/>
-    <mergeCell ref="L8:M8"/>
     <mergeCell ref="N6:P6"/>
-    <mergeCell ref="D11:AM11"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="D27:G27"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="L27:M27"/>
-    <mergeCell ref="N27:P27"/>
-    <mergeCell ref="A28:C28"/>
     <mergeCell ref="D28:G28"/>
     <mergeCell ref="H28:I28"/>
     <mergeCell ref="J28:K28"/>
@@ -3889,7 +3889,7 @@
     <mergeCell ref="N31:P31"/>
     <mergeCell ref="A32:C32"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>